<commit_message>
add tracking1,2, contact in report trial blance
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/tb.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/tb.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Trial Balance</t>
   </si>
@@ -24,6 +24,27 @@
   </si>
   <si>
     <t>As at {{fmt_date date}}</t>
+  </si>
+  <si>
+    <t>{{#if track_name}}</t>
+  </si>
+  <si>
+    <t>Tracking: {{track_name}}</t>
+  </si>
+  <si>
+    <t>{{/if}}</t>
+  </si>
+  <si>
+    <t>{{#if track2_name}}</t>
+  </si>
+  <si>
+    <t>Tracking-2: {{track2_name}}</t>
+  </si>
+  <si>
+    <t>{{#if contact_name}}</t>
+  </si>
+  <si>
+    <t>Contact: {{contact_name}}</t>
   </si>
   <si>
     <t>Account Code</t>
@@ -341,13 +362,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -406,256 +427,373 @@
       <c r="H4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" s="5" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" s="5" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="C15" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="F15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="G15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="H15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="9" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="B18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" s="12" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="11" t="s">
+      <c r="E21" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="F21" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="G21" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="H21" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="12" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" s="14" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" s="14" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" s="16" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" s="14" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-    </row>
-    <row r="21" s="14" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" s="17" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" s="14" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+    <row r="25" s="12" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="12" t="s">
         <v>35</v>
       </c>
+      <c r="F25" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" s="14" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" s="14" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" s="16" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" s="14" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" s="14" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" s="17" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" s="14" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="12">
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:H13"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>